<commit_message>
add xls files to complete assignment 8
</commit_message>
<xml_diff>
--- a/unit8-linear optimization/EvenStarFarm.xlsx
+++ b/unit8-linear optimization/EvenStarFarm.xlsx
@@ -1,15 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="1780" windowWidth="16920" windowHeight="15160" tabRatio="500"/>
+    <workbookView xWindow="45" yWindow="1785" windowWidth="16920" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$26:$D$33</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$C$41:$C$51</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$A$37</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$E$41:$E$51</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>EVEN' STAR ORGANIC PRODUCE</t>
   </si>
@@ -97,20 +129,56 @@
   </si>
   <si>
     <t>Objective: Maximize total profit</t>
+  </si>
+  <si>
+    <t>constraints</t>
+  </si>
+  <si>
+    <t>available</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LHS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RHS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;=</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>truck capacity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>restaurants limit</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSA customers limit</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="183" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -118,15 +186,33 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,8 +231,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -390,11 +482,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -405,10 +560,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -417,13 +572,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -472,12 +627,52 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="183" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -803,22 +998,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.75" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="25.625" customWidth="1"/>
+    <col min="5" max="5" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -827,14 +1023,14 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -843,14 +1039,14 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="16" thickBot="1">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" s="17" customFormat="1" ht="16" thickBot="1">
+    <row r="5" spans="1:7" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>2</v>
       </c>
@@ -867,7 +1063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -883,8 +1079,11 @@
       <c r="E6" s="5">
         <v>38.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="G6" s="38">
+        <v>713.47119327733526</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -900,8 +1099,11 @@
       <c r="E7" s="5">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7" s="38">
+        <v>331.49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -917,13 +1119,17 @@
       <c r="E8" s="5">
         <v>20.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8" s="38">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>76</v>
+        <f>10+76</f>
+        <v>86</v>
       </c>
       <c r="C9" s="4">
         <v>24</v>
@@ -934,8 +1140,11 @@
       <c r="E9" s="5">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" s="38">
+        <v>331.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -951,8 +1160,11 @@
       <c r="E10" s="5">
         <v>21.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10" s="38">
+        <v>552.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -968,8 +1180,11 @@
       <c r="E11" s="5">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11" s="38">
+        <v>565.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -985,8 +1200,11 @@
       <c r="E12" s="5">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="16" thickBot="1">
+      <c r="G12" s="38">
+        <v>673.47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
@@ -1002,22 +1220,25 @@
       <c r="E13" s="9">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="G13" s="38">
+        <v>673.47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1026,14 +1247,14 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="16" thickBot="1">
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" s="17" customFormat="1" ht="16" thickBot="1">
+    <row r="18" spans="1:5" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="15" t="s">
         <v>16</v>
@@ -1046,7 +1267,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1061,7 +1282,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="16" thickBot="1">
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -1076,21 +1297,21 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
         <v>21</v>
       </c>
@@ -1099,14 +1320,14 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="16" thickBot="1">
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" s="17" customFormat="1" ht="16" thickBot="1">
+    <row r="25" spans="1:5" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>2</v>
       </c>
@@ -1121,112 +1342,374 @@
       </c>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
+      <c r="B26" s="18">
+        <v>416</v>
+      </c>
+      <c r="C26" s="19">
+        <v>0</v>
+      </c>
+      <c r="D26" s="20">
+        <v>0</v>
+      </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
+      <c r="B27" s="21">
+        <v>0</v>
+      </c>
+      <c r="C27" s="22">
+        <v>608</v>
+      </c>
+      <c r="D27" s="23">
+        <v>0</v>
+      </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
+      <c r="B28" s="21">
+        <v>0</v>
+      </c>
+      <c r="C28" s="22">
+        <v>0</v>
+      </c>
+      <c r="D28" s="23">
+        <v>167</v>
+      </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
+      <c r="B29" s="21">
+        <v>0</v>
+      </c>
+      <c r="C29" s="22">
+        <v>86</v>
+      </c>
+      <c r="D29" s="23">
+        <v>0</v>
+      </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="23"/>
+      <c r="B30" s="21">
+        <v>0</v>
+      </c>
+      <c r="C30" s="22">
+        <v>72</v>
+      </c>
+      <c r="D30" s="23">
+        <v>0</v>
+      </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
+      <c r="B31" s="21">
+        <v>0</v>
+      </c>
+      <c r="C31" s="22">
+        <v>0</v>
+      </c>
+      <c r="D31" s="23">
+        <v>251</v>
+      </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
+      <c r="B32" s="21">
+        <v>0</v>
+      </c>
+      <c r="C32" s="22">
+        <v>0</v>
+      </c>
+      <c r="D32" s="23">
+        <v>107</v>
+      </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" ht="16" thickBot="1">
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
+      <c r="B33" s="24">
+        <v>58</v>
+      </c>
+      <c r="C33" s="25">
+        <v>0</v>
+      </c>
+      <c r="D33" s="26">
+        <v>75</v>
+      </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" ht="37" thickBot="1">
+    <row r="36" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="37">
+        <f>A37-49956.3917680672</f>
+        <v>713.47119327733526</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" ht="16" thickBot="1">
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <f>SUMPRODUCT(B26:D33,C6:E13) - B19*(SUM(B26:B33)/119) - B20 - C19*(SUMPRODUCT(C26:C33,D6:D13)/400) - C20 - D20</f>
-        <v>-8059.5</v>
+        <v>50669.862961344537</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C40" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="30">
+        <f>SUM(B26:D26)</f>
+        <v>416</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" s="30">
+        <f>B6</f>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" s="32"/>
+      <c r="B42" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="30">
+        <f t="shared" ref="C42:C48" si="0">SUM(B27:D27)</f>
+        <v>608</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="30">
+        <f t="shared" ref="E42:E48" si="1">B7</f>
+        <v>608</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" s="32"/>
+      <c r="B43" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="30">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" s="30">
+        <f t="shared" si="1"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" s="32"/>
+      <c r="B44" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="30">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="30">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="32"/>
+      <c r="B45" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="30">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" s="30">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" s="32"/>
+      <c r="B46" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="30">
+        <f t="shared" si="0"/>
+        <v>251</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" s="30">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" s="32"/>
+      <c r="B47" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="30">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="30">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="33"/>
+      <c r="B48" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="30">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="30">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" s="34"/>
+      <c r="C49" s="30">
+        <f>SUM(D26:D33)</f>
+        <v>600</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" s="30">
+        <f>600</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="34"/>
+      <c r="C50" s="30">
+        <f>SUM(B26:B33)/119</f>
+        <v>3.9831932773109244</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="36"/>
+      <c r="C51" s="30">
+        <f>SUMPRODUCT(C26:C33,D6:D13)/400</f>
+        <v>66.78</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="30">
+        <f>90</f>
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>